<commit_message>
added new comments and descriptiions
</commit_message>
<xml_diff>
--- a/Projet-Site Web-Grille de planification.xlsx
+++ b/Projet-Site Web-Grille de planification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ccnbca-my.sharepoint.com/personal/dimitri_viel_ccnb_ca/Documents/Prog1343/Lab1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f06159e0fb91e7d/Cybersecurity Year 1/ProjetGitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="79" documentId="8_{70D9F1CF-C19D-495D-9CA6-F522F37EBA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01FD7A3A-9F0C-4239-8D7D-CF227E972641}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -374,8 +374,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-1009]d/mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-1009]d/mmm/yy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -582,7 +582,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
@@ -626,13 +626,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -671,7 +671,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -686,12 +686,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -710,22 +719,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
+    <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1004,36 +1004,36 @@
   </sheetPr>
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="59.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="72.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="72.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>2</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>3</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>4</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>5</v>
       </c>
@@ -1071,7 +1071,7 @@
       <c r="C8" s="33"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>6</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>7</v>
       </c>
@@ -1089,57 +1089,57 @@
       <c r="C10" s="33"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="38"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36" t="s">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="38"/>
+      <c r="C14" s="41"/>
       <c r="D14" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="14">
         <v>45240</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>14</v>
       </c>
@@ -1149,31 +1149,31 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
+    <row r="21" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>17</v>
       </c>
@@ -1183,27 +1183,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="35" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-    </row>
-    <row r="26" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+    </row>
+    <row r="26" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
         <v>19</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>20</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
         <v>21</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
         <v>22</v>
       </c>
@@ -1243,37 +1243,37 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="9"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="35" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="42" t="s">
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="44"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
       <c r="B34" s="24" t="s">
         <v>25</v>
@@ -1281,7 +1281,7 @@
       <c r="C34" s="25"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="24" t="s">
         <v>26</v>
@@ -1291,7 +1291,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="24" t="s">
         <v>27</v>
@@ -1301,7 +1301,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
       <c r="B37" s="24" t="s">
         <v>28</v>
@@ -1311,7 +1311,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
         <v>29</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
         <v>30</v>
       </c>
@@ -1331,56 +1331,56 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="40"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="35" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
       <c r="D43" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="45" t="s">
+    <row r="44" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
       <c r="D44" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="45" t="s">
+    <row r="45" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
       <c r="D45" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
         <v>35</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
         <v>36</v>
       </c>
@@ -1400,25 +1400,25 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
       <c r="B48" s="19"/>
       <c r="C48" s="19"/>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
       <c r="B49" s="19"/>
       <c r="C49" s="19"/>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="35" t="s">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="35"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-    </row>
-    <row r="51" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+    </row>
+    <row r="51" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
         <v>38</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
         <v>39</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="21"/>
       <c r="B53" s="26">
         <v>1</v>
@@ -1450,7 +1450,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="26">
         <v>2</v>
@@ -1462,7 +1462,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="26">
         <v>3</v>
@@ -1474,7 +1474,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
       <c r="B56" s="26">
         <v>4</v>
@@ -1486,7 +1486,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21"/>
       <c r="B57" s="26">
         <v>5</v>
@@ -1498,7 +1498,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
       <c r="B58" s="26">
         <v>6</v>
@@ -1510,7 +1510,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
       <c r="B59" s="26">
         <v>7</v>
@@ -1522,7 +1522,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
       <c r="B60" s="26">
         <v>8</v>
@@ -1534,7 +1534,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="21"/>
       <c r="B61" s="26">
         <v>9</v>
@@ -1546,7 +1546,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="21"/>
       <c r="B62" s="26">
         <v>10</v>
@@ -1554,7 +1554,7 @@
       <c r="C62" s="20"/>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="21"/>
       <c r="B63" s="26">
         <v>11</v>
@@ -1562,7 +1562,7 @@
       <c r="C63" s="20"/>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="21"/>
       <c r="B64" s="26">
         <v>12</v>
@@ -1570,7 +1570,7 @@
       <c r="C64" s="20"/>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="33" t="s">
         <v>41</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="33" t="s">
         <v>42</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="33" t="s">
         <v>43</v>
       </c>
@@ -1600,55 +1600,55 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
       <c r="B68" s="19"/>
       <c r="C68" s="19"/>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
       <c r="B69" s="19"/>
       <c r="C69" s="19"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="35" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B70" s="35"/>
-      <c r="C70" s="35"/>
-      <c r="D70" s="35"/>
-    </row>
-    <row r="71" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="36" t="s">
+      <c r="B70" s="37"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="37"/>
+    </row>
+    <row r="71" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B71" s="37"/>
-      <c r="C71" s="38"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="41"/>
       <c r="D71" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="36" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B72" s="37"/>
-      <c r="C72" s="38"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="41"/>
       <c r="D72" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="36" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="37"/>
-      <c r="C73" s="38"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="41"/>
       <c r="D73" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="33" t="s">
         <v>48</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="33" t="s">
         <v>49</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
         <v>50</v>
       </c>
@@ -1678,20 +1678,20 @@
         <v>66</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="19"/>
       <c r="B77" s="19"/>
       <c r="C77" s="19"/>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="35" t="s">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-    </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
+    </row>
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="33" t="s">
         <v>52</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="33" t="s">
         <v>53</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="22"/>
       <c r="B81" s="27" t="s">
         <v>55</v>
@@ -1721,7 +1721,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="22"/>
       <c r="B82" s="27" t="s">
         <v>56</v>
@@ -1731,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="22"/>
       <c r="B83" s="27" t="s">
         <v>57</v>
@@ -1741,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="22"/>
       <c r="B84" s="27" t="s">
         <v>58</v>
@@ -1751,7 +1751,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="22"/>
       <c r="B85" s="27" t="s">
         <v>59</v>
@@ -1761,7 +1761,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="22"/>
       <c r="B86" s="27" t="s">
         <v>60</v>
@@ -1771,7 +1771,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
       <c r="B87" s="27" t="s">
         <v>61</v>
@@ -1781,7 +1781,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="33" t="s">
         <v>62</v>
       </c>
@@ -1791,20 +1791,55 @@
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="C91" s="32" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C98" s="18"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A88:C88"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A47:C47"/>
@@ -1821,41 +1856,6 @@
     <mergeCell ref="A51:C51"/>
     <mergeCell ref="A52:C52"/>
     <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" xr:uid="{6EFAE0B5-110C-4B79-958F-9FA5C5BB2F93}"/>

</xml_diff>